<commit_message>
added additonal information output
</commit_message>
<xml_diff>
--- a/Excel/2021.08.08.xlsx
+++ b/Excel/2021.08.08.xlsx
@@ -13267,10 +13267,10 @@
         <v>82281</v>
       </c>
       <c r="F2" t="n">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="G2" t="n">
-        <v>82308</v>
+        <v>82331</v>
       </c>
     </row>
     <row r="3">
@@ -13294,10 +13294,10 @@
         <v>80258</v>
       </c>
       <c r="F3" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G3" t="n">
-        <v>80297</v>
+        <v>80330</v>
       </c>
     </row>
     <row r="4">
@@ -13321,10 +13321,10 @@
         <v>60500</v>
       </c>
       <c r="F4" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G4" t="n">
-        <v>60524</v>
+        <v>60536</v>
       </c>
     </row>
     <row r="5">
@@ -13348,10 +13348,10 @@
         <v>40192</v>
       </c>
       <c r="F5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" t="n">
-        <v>40200</v>
+        <v>40203</v>
       </c>
     </row>
     <row r="6">
@@ -13375,10 +13375,10 @@
         <v>35222</v>
       </c>
       <c r="F6" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G6" t="n">
-        <v>35245</v>
+        <v>35253</v>
       </c>
     </row>
     <row r="7">
@@ -13402,10 +13402,10 @@
         <v>27856</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G7" t="n">
-        <v>27864</v>
+        <v>27869</v>
       </c>
     </row>
     <row r="8">
@@ -13429,10 +13429,10 @@
         <v>34627</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>34637</v>
+        <v>34643</v>
       </c>
     </row>
     <row r="9">
@@ -13456,10 +13456,10 @@
         <v>27088</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>27090</v>
+        <v>27093</v>
       </c>
     </row>
     <row r="10">
@@ -13483,10 +13483,10 @@
         <v>26748</v>
       </c>
       <c r="F10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>26752</v>
+        <v>26757</v>
       </c>
     </row>
     <row r="11">
@@ -13537,10 +13537,10 @@
         <v>27437</v>
       </c>
       <c r="F12" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G12" t="n">
-        <v>27458</v>
+        <v>27475</v>
       </c>
     </row>
     <row r="13">
@@ -13564,10 +13564,10 @@
         <v>26201</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G13" t="n">
-        <v>26202</v>
+        <v>26214</v>
       </c>
     </row>
     <row r="14">
@@ -13618,10 +13618,10 @@
         <v>25367</v>
       </c>
       <c r="F15" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G15" t="n">
-        <v>25391</v>
+        <v>25410</v>
       </c>
     </row>
     <row r="16">
@@ -13645,10 +13645,10 @@
         <v>21238</v>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G16" t="n">
-        <v>21248</v>
+        <v>21253</v>
       </c>
     </row>
     <row r="17">
@@ -13672,10 +13672,10 @@
         <v>33341</v>
       </c>
       <c r="F17" t="n">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="G17" t="n">
-        <v>33417</v>
+        <v>33462</v>
       </c>
     </row>
     <row r="18">
@@ -13699,10 +13699,10 @@
         <v>21588</v>
       </c>
       <c r="F18" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G18" t="n">
-        <v>21596</v>
+        <v>21609</v>
       </c>
     </row>
     <row r="19">
@@ -13726,10 +13726,10 @@
         <v>19591</v>
       </c>
       <c r="F19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" t="n">
-        <v>19597</v>
+        <v>19596</v>
       </c>
     </row>
     <row r="20">
@@ -13753,10 +13753,10 @@
         <v>18203</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G20" t="n">
-        <v>18204</v>
+        <v>18209</v>
       </c>
     </row>
     <row r="21" ht="28.8" customHeight="1">
@@ -13780,10 +13780,10 @@
         <v>19752</v>
       </c>
       <c r="F21" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G21" t="n">
-        <v>19759</v>
+        <v>19768</v>
       </c>
     </row>
     <row r="22">
@@ -13807,10 +13807,10 @@
         <v>18912</v>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G22" t="n">
-        <v>18923</v>
+        <v>18937</v>
       </c>
     </row>
     <row r="23">
@@ -13834,10 +13834,10 @@
         <v>17318</v>
       </c>
       <c r="F23" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G23" t="n">
-        <v>17327</v>
+        <v>17331</v>
       </c>
     </row>
     <row r="24">
@@ -13861,10 +13861,10 @@
         <v>19008</v>
       </c>
       <c r="F24" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G24" t="n">
-        <v>19026</v>
+        <v>19042</v>
       </c>
     </row>
     <row r="25">
@@ -13888,10 +13888,10 @@
         <v>16196</v>
       </c>
       <c r="F25" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G25" t="n">
-        <v>16207</v>
+        <v>16210</v>
       </c>
     </row>
     <row r="26">
@@ -13915,10 +13915,10 @@
         <v>14788</v>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>14790</v>
+        <v>14792</v>
       </c>
     </row>
     <row r="27">
@@ -13942,10 +13942,10 @@
         <v>15213</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G27" t="n">
-        <v>15217</v>
+        <v>15219</v>
       </c>
     </row>
     <row r="28">
@@ -13969,10 +13969,10 @@
         <v>14419</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G28" t="n">
-        <v>14421</v>
+        <v>14423</v>
       </c>
     </row>
     <row r="29">
@@ -13996,10 +13996,10 @@
         <v>13095</v>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G29" t="n">
-        <v>13100</v>
+        <v>13103</v>
       </c>
     </row>
     <row r="30">
@@ -14023,10 +14023,10 @@
         <v>13006</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>13006</v>
+        <v>13007</v>
       </c>
     </row>
     <row r="31">
@@ -14050,10 +14050,10 @@
         <v>13760</v>
       </c>
       <c r="F31" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31" t="n">
-        <v>13768</v>
+        <v>13769</v>
       </c>
     </row>
     <row r="32">
@@ -14077,10 +14077,10 @@
         <v>11390</v>
       </c>
       <c r="F32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G32" t="n">
-        <v>11394</v>
+        <v>11395</v>
       </c>
     </row>
     <row r="33">
@@ -14131,10 +14131,10 @@
         <v>12689</v>
       </c>
       <c r="F34" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G34" t="n">
-        <v>12692</v>
+        <v>12696</v>
       </c>
     </row>
     <row r="35">
@@ -14158,10 +14158,10 @@
         <v>13040</v>
       </c>
       <c r="F35" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G35" t="n">
-        <v>13050</v>
+        <v>13048</v>
       </c>
     </row>
     <row r="36">
@@ -14212,10 +14212,10 @@
         <v>11072</v>
       </c>
       <c r="F37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G37" t="n">
-        <v>11076</v>
+        <v>11077</v>
       </c>
     </row>
     <row r="38">
@@ -14266,10 +14266,10 @@
         <v>10447</v>
       </c>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>10449</v>
+        <v>10448</v>
       </c>
     </row>
     <row r="40">
@@ -14293,10 +14293,10 @@
         <v>11068</v>
       </c>
       <c r="F40" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G40" t="n">
-        <v>11066</v>
+        <v>11067</v>
       </c>
     </row>
     <row r="41">
@@ -14320,10 +14320,10 @@
         <v>10425</v>
       </c>
       <c r="F41" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G41" t="n">
-        <v>10422</v>
+        <v>10424</v>
       </c>
     </row>
     <row r="42">
@@ -14347,10 +14347,10 @@
         <v>11730</v>
       </c>
       <c r="F42" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G42" t="n">
-        <v>11739</v>
+        <v>11746</v>
       </c>
     </row>
     <row r="43">
@@ -14374,10 +14374,10 @@
         <v>9957</v>
       </c>
       <c r="F43" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G43" t="n">
-        <v>9965</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="44">
@@ -14428,10 +14428,10 @@
         <v>10647</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G45" t="n">
-        <v>10648</v>
+        <v>10653</v>
       </c>
     </row>
     <row r="46">
@@ -14509,10 +14509,10 @@
         <v>9877</v>
       </c>
       <c r="F48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G48" t="n">
-        <v>9881</v>
+        <v>9882</v>
       </c>
     </row>
     <row r="49">
@@ -14583,10 +14583,10 @@
         <v>13128</v>
       </c>
       <c r="F52" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="G52" t="n">
-        <v>13147</v>
+        <v>13166</v>
       </c>
     </row>
     <row r="53">
@@ -14606,10 +14606,10 @@
         <v>9741</v>
       </c>
       <c r="F53" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" t="n">
-        <v>9750</v>
+        <v>9752</v>
       </c>
     </row>
     <row r="54" ht="28.8" customHeight="1">
@@ -14629,10 +14629,10 @@
         <v>9363</v>
       </c>
       <c r="F54" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G54" t="n">
-        <v>9371</v>
+        <v>9379</v>
       </c>
     </row>
     <row r="55">
@@ -27546,10 +27546,10 @@
         <v>1590816</v>
       </c>
       <c r="T32" t="n">
-        <v>647</v>
+        <v>1117</v>
       </c>
       <c r="U32" t="n">
-        <v>1591463</v>
+        <v>1591933</v>
       </c>
     </row>
     <row r="33">
@@ -38235,10 +38235,10 @@
         <v>182192</v>
       </c>
       <c r="F2" t="n">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="G2" t="n">
-        <v>182243</v>
+        <v>182273</v>
       </c>
     </row>
     <row r="3">
@@ -38262,10 +38262,10 @@
         <v>156852</v>
       </c>
       <c r="F3" t="n">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="G3" t="n">
-        <v>156909</v>
+        <v>156953</v>
       </c>
     </row>
     <row r="4">
@@ -38289,10 +38289,10 @@
         <v>154699</v>
       </c>
       <c r="F4" t="n">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G4" t="n">
-        <v>154748</v>
+        <v>154760</v>
       </c>
     </row>
     <row r="5">
@@ -38316,10 +38316,10 @@
         <v>136974</v>
       </c>
       <c r="F5" t="n">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="G5" t="n">
-        <v>137024</v>
+        <v>137047</v>
       </c>
     </row>
     <row r="6">
@@ -38343,10 +38343,10 @@
         <v>131662</v>
       </c>
       <c r="F6" t="n">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="G6" t="n">
-        <v>131704</v>
+        <v>131747</v>
       </c>
     </row>
     <row r="7">
@@ -38370,10 +38370,10 @@
         <v>128931</v>
       </c>
       <c r="F7" t="n">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="G7" t="n">
-        <v>129009</v>
+        <v>129073</v>
       </c>
     </row>
     <row r="8">
@@ -38397,10 +38397,10 @@
         <v>90347</v>
       </c>
       <c r="F8" t="n">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="G8" t="n">
-        <v>90368</v>
+        <v>90386</v>
       </c>
     </row>
     <row r="9">
@@ -38424,10 +38424,10 @@
         <v>80957</v>
       </c>
       <c r="F9" t="n">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G9" t="n">
-        <v>81004</v>
+        <v>81023</v>
       </c>
     </row>
     <row r="10">
@@ -38451,10 +38451,10 @@
         <v>61922</v>
       </c>
       <c r="F10" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G10" t="n">
-        <v>61965</v>
+        <v>61978</v>
       </c>
     </row>
     <row r="11">
@@ -38478,10 +38478,10 @@
         <v>76059</v>
       </c>
       <c r="F11" t="n">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="G11" t="n">
-        <v>76103</v>
+        <v>76123</v>
       </c>
     </row>
     <row r="12">
@@ -38505,10 +38505,10 @@
         <v>72662</v>
       </c>
       <c r="F12" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G12" t="n">
-        <v>72687</v>
+        <v>72702</v>
       </c>
     </row>
     <row r="13">
@@ -38532,10 +38532,10 @@
         <v>71716</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>71722</v>
+        <v>71726</v>
       </c>
     </row>
     <row r="14">
@@ -38559,10 +38559,10 @@
         <v>59073</v>
       </c>
       <c r="F14" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G14" t="n">
-        <v>59096</v>
+        <v>59104</v>
       </c>
     </row>
     <row r="15">
@@ -38586,10 +38586,10 @@
         <v>67115</v>
       </c>
       <c r="F15" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G15" t="n">
-        <v>67135</v>
+        <v>67141</v>
       </c>
     </row>
     <row r="16">
@@ -38613,10 +38613,10 @@
         <v>59708</v>
       </c>
       <c r="F16" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G16" t="n">
-        <v>59716</v>
+        <v>59731</v>
       </c>
     </row>
     <row r="17">
@@ -38640,10 +38640,10 @@
         <v>64096</v>
       </c>
       <c r="F17" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G17" t="n">
-        <v>64112</v>
+        <v>64129</v>
       </c>
     </row>
     <row r="18">
@@ -38667,10 +38667,10 @@
         <v>62058</v>
       </c>
       <c r="F18" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G18" t="n">
-        <v>62079</v>
+        <v>62091</v>
       </c>
     </row>
     <row r="19">
@@ -38694,10 +38694,10 @@
         <v>64774</v>
       </c>
       <c r="F19" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G19" t="n">
-        <v>64794</v>
+        <v>64809</v>
       </c>
     </row>
     <row r="20">
@@ -38721,10 +38721,10 @@
         <v>62230</v>
       </c>
       <c r="F20" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G20" t="n">
-        <v>62242</v>
+        <v>62246</v>
       </c>
     </row>
     <row r="21">
@@ -38748,10 +38748,10 @@
         <v>46155</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G21" t="n">
-        <v>46158</v>
+        <v>46172</v>
       </c>
     </row>
     <row r="22">
@@ -38775,10 +38775,10 @@
         <v>57919</v>
       </c>
       <c r="F22" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G22" t="n">
-        <v>57937</v>
+        <v>57953</v>
       </c>
     </row>
     <row r="23">
@@ -38802,10 +38802,10 @@
         <v>49731</v>
       </c>
       <c r="F23" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G23" t="n">
-        <v>49750</v>
+        <v>49755</v>
       </c>
     </row>
     <row r="24">
@@ -38829,10 +38829,10 @@
         <v>51897</v>
       </c>
       <c r="F24" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G24" t="n">
-        <v>51907</v>
+        <v>51911</v>
       </c>
     </row>
     <row r="25">
@@ -38856,10 +38856,10 @@
         <v>55006</v>
       </c>
       <c r="F25" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G25" t="n">
-        <v>55015</v>
+        <v>55020</v>
       </c>
     </row>
     <row r="26">
@@ -38883,10 +38883,10 @@
         <v>48788</v>
       </c>
       <c r="F26" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G26" t="n">
-        <v>48802</v>
+        <v>48806</v>
       </c>
     </row>
     <row r="27">
@@ -38910,10 +38910,10 @@
         <v>49641</v>
       </c>
       <c r="F27" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G27" t="n">
-        <v>49649</v>
+        <v>49652</v>
       </c>
     </row>
     <row r="28">
@@ -38937,10 +38937,10 @@
         <v>49192</v>
       </c>
       <c r="F28" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G28" t="n">
-        <v>49209</v>
+        <v>49216</v>
       </c>
     </row>
     <row r="29">
@@ -38964,10 +38964,10 @@
         <v>44983</v>
       </c>
       <c r="F29" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G29" t="n">
-        <v>44998</v>
+        <v>45004</v>
       </c>
     </row>
     <row r="30">
@@ -38991,10 +38991,10 @@
         <v>42101</v>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G30" t="n">
-        <v>42111</v>
+        <v>42119</v>
       </c>
     </row>
     <row r="31">
@@ -39018,10 +39018,10 @@
         <v>41179</v>
       </c>
       <c r="F31" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G31" t="n">
-        <v>41190</v>
+        <v>41192</v>
       </c>
     </row>
     <row r="32">
@@ -39045,10 +39045,10 @@
         <v>42113</v>
       </c>
       <c r="F32" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G32" t="n">
-        <v>42131</v>
+        <v>42147</v>
       </c>
     </row>
     <row r="33">
@@ -39072,10 +39072,10 @@
         <v>44113</v>
       </c>
       <c r="F33" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G33" t="n">
-        <v>44119</v>
+        <v>44123</v>
       </c>
     </row>
     <row r="34">
@@ -39099,10 +39099,10 @@
         <v>43717</v>
       </c>
       <c r="F34" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G34" t="n">
-        <v>43727</v>
+        <v>43725</v>
       </c>
     </row>
     <row r="35">
@@ -39126,10 +39126,10 @@
         <v>49725</v>
       </c>
       <c r="F35" t="n">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="G35" t="n">
-        <v>49779</v>
+        <v>49802</v>
       </c>
     </row>
     <row r="36">
@@ -39153,10 +39153,10 @@
         <v>42671</v>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G36" t="n">
-        <v>42681</v>
+        <v>42687</v>
       </c>
     </row>
     <row r="37">
@@ -39180,10 +39180,10 @@
         <v>38829</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G37" t="n">
-        <v>38839</v>
+        <v>38849</v>
       </c>
     </row>
     <row r="38">
@@ -39207,10 +39207,10 @@
         <v>40835</v>
       </c>
       <c r="F38" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G38" t="n">
-        <v>40857</v>
+        <v>40872</v>
       </c>
     </row>
     <row r="39" ht="28.8" customHeight="1">
@@ -39234,10 +39234,10 @@
         <v>35920</v>
       </c>
       <c r="F39" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G39" t="n">
-        <v>35924</v>
+        <v>35930</v>
       </c>
     </row>
     <row r="40">
@@ -39261,10 +39261,10 @@
         <v>33367</v>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G40" t="n">
-        <v>33370</v>
+        <v>33371</v>
       </c>
     </row>
     <row r="41">
@@ -39288,10 +39288,10 @@
         <v>32636</v>
       </c>
       <c r="F41" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G41" t="n">
-        <v>32642</v>
+        <v>32640</v>
       </c>
     </row>
     <row r="42">
@@ -39315,10 +39315,10 @@
         <v>29514</v>
       </c>
       <c r="F42" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G42" t="n">
-        <v>29520</v>
+        <v>29527</v>
       </c>
     </row>
     <row r="43" ht="28.8" customHeight="1">
@@ -39342,10 +39342,10 @@
         <v>34750</v>
       </c>
       <c r="F43" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G43" t="n">
-        <v>34766</v>
+        <v>34782</v>
       </c>
     </row>
     <row r="44">
@@ -39369,10 +39369,10 @@
         <v>29081</v>
       </c>
       <c r="F44" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G44" t="n">
-        <v>29099</v>
+        <v>29109</v>
       </c>
     </row>
     <row r="45">
@@ -39396,10 +39396,10 @@
         <v>28468</v>
       </c>
       <c r="F45" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G45" t="n">
-        <v>28475</v>
+        <v>28478</v>
       </c>
     </row>
     <row r="46">
@@ -39450,10 +39450,10 @@
         <v>30626</v>
       </c>
       <c r="F47" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G47" t="n">
-        <v>30648</v>
+        <v>30657</v>
       </c>
     </row>
     <row r="48" ht="28.8" customHeight="1">
@@ -39477,10 +39477,10 @@
         <v>29743</v>
       </c>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G48" t="n">
-        <v>29745</v>
+        <v>29750</v>
       </c>
     </row>
     <row r="49">
@@ -39531,10 +39531,10 @@
         <v>29451</v>
       </c>
       <c r="F50" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G50" t="n">
-        <v>29461</v>
+        <v>29464</v>
       </c>
     </row>
     <row r="51">
@@ -39558,10 +39558,10 @@
         <v>31187</v>
       </c>
       <c r="F51" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G51" t="n">
-        <v>31199</v>
+        <v>31206</v>
       </c>
     </row>
     <row r="52">
@@ -43350,10 +43350,10 @@
         <v>8.84</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>-0.009999999999999787</v>
       </c>
       <c r="S16" t="n">
-        <v>8.84</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="17">
@@ -44421,10 +44421,10 @@
         <v>8.75</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>0.009999999999999787</v>
       </c>
       <c r="S33" t="n">
-        <v>8.75</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="34">
@@ -44925,10 +44925,10 @@
         <v>8.699999999999999</v>
       </c>
       <c r="R41" t="n">
-        <v>0.01000000000000156</v>
+        <v>0</v>
       </c>
       <c r="S41" t="n">
-        <v>8.710000000000001</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="42">
@@ -45104,10 +45104,10 @@
         <v>8.68</v>
       </c>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>0.009999999999999787</v>
       </c>
       <c r="S44" t="n">
-        <v>8.68</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="45">
@@ -45768,10 +45768,10 @@
         <v>8.710000000000001</v>
       </c>
       <c r="R60" t="n">
-        <v>-0.01000000000000156</v>
+        <v>-0.02000000000000135</v>
       </c>
       <c r="S60" t="n">
-        <v>8.699999999999999</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="61">
@@ -55462,10 +55462,10 @@
         <v>498684</v>
       </c>
       <c r="N2" t="n">
-        <v>174</v>
+        <v>307</v>
       </c>
       <c r="O2" t="n">
-        <v>498858</v>
+        <v>498991</v>
       </c>
     </row>
     <row r="3">
@@ -55513,10 +55513,10 @@
         <v>410367</v>
       </c>
       <c r="N3" t="n">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="O3" t="n">
-        <v>410499</v>
+        <v>410594</v>
       </c>
     </row>
     <row r="4">
@@ -55564,10 +55564,10 @@
         <v>350549</v>
       </c>
       <c r="N4" t="n">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="O4" t="n">
-        <v>350610</v>
+        <v>350644</v>
       </c>
     </row>
     <row r="5">
@@ -55615,10 +55615,10 @@
         <v>427691</v>
       </c>
       <c r="N5" t="n">
-        <v>174</v>
+        <v>292</v>
       </c>
       <c r="O5" t="n">
-        <v>427865</v>
+        <v>427983</v>
       </c>
     </row>
     <row r="6">
@@ -55666,10 +55666,10 @@
         <v>370484</v>
       </c>
       <c r="N6" t="n">
-        <v>117</v>
+        <v>189</v>
       </c>
       <c r="O6" t="n">
-        <v>370601</v>
+        <v>370673</v>
       </c>
     </row>
     <row r="7">
@@ -55717,10 +55717,10 @@
         <v>329490</v>
       </c>
       <c r="N7" t="n">
-        <v>114</v>
+        <v>187</v>
       </c>
       <c r="O7" t="n">
-        <v>329604</v>
+        <v>329677</v>
       </c>
     </row>
     <row r="8">
@@ -55768,10 +55768,10 @@
         <v>315804</v>
       </c>
       <c r="N8" t="n">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="O8" t="n">
-        <v>315913</v>
+        <v>315955</v>
       </c>
     </row>
     <row r="9">
@@ -55819,10 +55819,10 @@
         <v>288873</v>
       </c>
       <c r="N9" t="n">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="O9" t="n">
-        <v>288978</v>
+        <v>289026</v>
       </c>
     </row>
     <row r="10">
@@ -55870,10 +55870,10 @@
         <v>332512</v>
       </c>
       <c r="N10" t="n">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="O10" t="n">
-        <v>332646</v>
+        <v>332744</v>
       </c>
     </row>
     <row r="11">
@@ -55921,10 +55921,10 @@
         <v>242433</v>
       </c>
       <c r="N11" t="n">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="O11" t="n">
-        <v>242456</v>
+        <v>242473</v>
       </c>
     </row>
     <row r="12">
@@ -55972,10 +55972,10 @@
         <v>236896</v>
       </c>
       <c r="N12" t="n">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="O12" t="n">
-        <v>236945</v>
+        <v>236976</v>
       </c>
     </row>
     <row r="13">
@@ -56023,10 +56023,10 @@
         <v>276172</v>
       </c>
       <c r="N13" t="n">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="O13" t="n">
-        <v>276293</v>
+        <v>276369</v>
       </c>
     </row>
     <row r="14">
@@ -56074,10 +56074,10 @@
         <v>219287</v>
       </c>
       <c r="N14" t="n">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="O14" t="n">
-        <v>219351</v>
+        <v>219406</v>
       </c>
     </row>
     <row r="15">
@@ -56125,10 +56125,10 @@
         <v>259872</v>
       </c>
       <c r="N15" t="n">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="O15" t="n">
-        <v>259955</v>
+        <v>260006</v>
       </c>
     </row>
     <row r="16">
@@ -56176,10 +56176,10 @@
         <v>210465</v>
       </c>
       <c r="N16" t="n">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="O16" t="n">
-        <v>210528</v>
+        <v>210568</v>
       </c>
     </row>
     <row r="17">
@@ -56227,10 +56227,10 @@
         <v>195953</v>
       </c>
       <c r="N17" t="n">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="O17" t="n">
-        <v>195998</v>
+        <v>196035</v>
       </c>
     </row>
     <row r="18">
@@ -56278,10 +56278,10 @@
         <v>234478</v>
       </c>
       <c r="N18" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="O18" t="n">
-        <v>234548</v>
+        <v>234608</v>
       </c>
     </row>
     <row r="19">
@@ -56329,10 +56329,10 @@
         <v>172139</v>
       </c>
       <c r="N19" t="n">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="O19" t="n">
-        <v>172160</v>
+        <v>172173</v>
       </c>
     </row>
     <row r="20">
@@ -56380,10 +56380,10 @@
         <v>160430</v>
       </c>
       <c r="N20" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="O20" t="n">
-        <v>160444</v>
+        <v>160458</v>
       </c>
     </row>
     <row r="21">
@@ -56431,10 +56431,10 @@
         <v>170998</v>
       </c>
       <c r="N21" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="O21" t="n">
-        <v>171033</v>
+        <v>171053</v>
       </c>
     </row>
     <row r="22">
@@ -56482,10 +56482,10 @@
         <v>167648</v>
       </c>
       <c r="N22" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="O22" t="n">
-        <v>167684</v>
+        <v>167697</v>
       </c>
     </row>
     <row r="23">
@@ -56533,10 +56533,10 @@
         <v>211231</v>
       </c>
       <c r="N23" t="n">
-        <v>104</v>
+        <v>175</v>
       </c>
       <c r="O23" t="n">
-        <v>211335</v>
+        <v>211406</v>
       </c>
     </row>
     <row r="24">
@@ -56584,10 +56584,10 @@
         <v>245355</v>
       </c>
       <c r="N24" t="n">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="O24" t="n">
-        <v>245522</v>
+        <v>245648</v>
       </c>
     </row>
     <row r="25">
@@ -56635,10 +56635,10 @@
         <v>155182</v>
       </c>
       <c r="N25" t="n">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="O25" t="n">
-        <v>155210</v>
+        <v>155228</v>
       </c>
     </row>
     <row r="26">
@@ -56686,10 +56686,10 @@
         <v>147936</v>
       </c>
       <c r="N26" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="O26" t="n">
-        <v>147978</v>
+        <v>147996</v>
       </c>
     </row>
     <row r="27">
@@ -56737,10 +56737,10 @@
         <v>145222</v>
       </c>
       <c r="N27" t="n">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="O27" t="n">
-        <v>145247</v>
+        <v>145268</v>
       </c>
     </row>
     <row r="28">
@@ -56788,10 +56788,10 @@
         <v>148413</v>
       </c>
       <c r="N28" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O28" t="n">
-        <v>148435</v>
+        <v>148457</v>
       </c>
     </row>
     <row r="29">
@@ -56839,10 +56839,10 @@
         <v>181133</v>
       </c>
       <c r="N29" t="n">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="O29" t="n">
-        <v>181213</v>
+        <v>181285</v>
       </c>
     </row>
     <row r="30">
@@ -56890,10 +56890,10 @@
         <v>145539</v>
       </c>
       <c r="N30" t="n">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="O30" t="n">
-        <v>145577</v>
+        <v>145604</v>
       </c>
     </row>
     <row r="31">
@@ -56941,10 +56941,10 @@
         <v>136226</v>
       </c>
       <c r="N31" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="O31" t="n">
-        <v>136246</v>
+        <v>136256</v>
       </c>
     </row>
     <row r="32">
@@ -56992,10 +56992,10 @@
         <v>140890</v>
       </c>
       <c r="N32" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="O32" t="n">
-        <v>140920</v>
+        <v>140950</v>
       </c>
     </row>
     <row r="33">
@@ -57043,10 +57043,10 @@
         <v>132482</v>
       </c>
       <c r="N33" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O33" t="n">
-        <v>132511</v>
+        <v>132526</v>
       </c>
     </row>
     <row r="34">
@@ -57094,10 +57094,10 @@
         <v>132160</v>
       </c>
       <c r="N34" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="O34" t="n">
-        <v>132176</v>
+        <v>132194</v>
       </c>
     </row>
     <row r="35">
@@ -57145,10 +57145,10 @@
         <v>129542</v>
       </c>
       <c r="N35" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="O35" t="n">
-        <v>129559</v>
+        <v>129573</v>
       </c>
     </row>
     <row r="36">
@@ -57196,10 +57196,10 @@
         <v>134077</v>
       </c>
       <c r="N36" t="n">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="O36" t="n">
-        <v>134109</v>
+        <v>134130</v>
       </c>
     </row>
     <row r="37">
@@ -57247,10 +57247,10 @@
         <v>143656</v>
       </c>
       <c r="N37" t="n">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="O37" t="n">
-        <v>143693</v>
+        <v>143709</v>
       </c>
     </row>
     <row r="38" ht="28.8" customHeight="1">
@@ -57298,10 +57298,10 @@
         <v>174619</v>
       </c>
       <c r="N38" t="n">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="O38" t="n">
-        <v>174702</v>
+        <v>174753</v>
       </c>
     </row>
     <row r="39">
@@ -57349,10 +57349,10 @@
         <v>254746</v>
       </c>
       <c r="N39" t="n">
-        <v>210</v>
+        <v>345</v>
       </c>
       <c r="O39" t="n">
-        <v>254956</v>
+        <v>255091</v>
       </c>
     </row>
     <row r="40">
@@ -57400,10 +57400,10 @@
         <v>146409</v>
       </c>
       <c r="N40" t="n">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="O40" t="n">
-        <v>146458</v>
+        <v>146500</v>
       </c>
     </row>
     <row r="41">
@@ -57451,10 +57451,10 @@
         <v>148693</v>
       </c>
       <c r="N41" t="n">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="O41" t="n">
-        <v>148758</v>
+        <v>148798</v>
       </c>
     </row>
     <row r="42">
@@ -57502,10 +57502,10 @@
         <v>129373</v>
       </c>
       <c r="N42" t="n">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="O42" t="n">
-        <v>129402</v>
+        <v>129428</v>
       </c>
     </row>
     <row r="43" ht="28.8" customHeight="1">
@@ -57553,10 +57553,10 @@
         <v>160649</v>
       </c>
       <c r="N43" t="n">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="O43" t="n">
-        <v>160770</v>
+        <v>160836</v>
       </c>
     </row>
     <row r="44">
@@ -57641,10 +57641,10 @@
         <v>147019</v>
       </c>
       <c r="N45" t="n">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="O45" t="n">
-        <v>147085</v>
+        <v>147135</v>
       </c>
     </row>
     <row r="46">
@@ -57729,10 +57729,10 @@
         <v>161604</v>
       </c>
       <c r="N47" t="n">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="O47" t="n">
-        <v>161680</v>
+        <v>161723</v>
       </c>
     </row>
     <row r="48">
@@ -57895,10 +57895,10 @@
         <v>149646</v>
       </c>
       <c r="N51" t="n">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="O51" t="n">
-        <v>149707</v>
+        <v>149756</v>
       </c>
     </row>
     <row r="52">
@@ -57930,10 +57930,10 @@
         <v>258748</v>
       </c>
       <c r="N52" t="n">
-        <v>403</v>
+        <v>627</v>
       </c>
       <c r="O52" t="n">
-        <v>259151</v>
+        <v>259375</v>
       </c>
     </row>
     <row r="53" ht="28.8" customHeight="1">
@@ -57965,10 +57965,10 @@
         <v>145239</v>
       </c>
       <c r="N53" t="n">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="O53" t="n">
-        <v>145343</v>
+        <v>145409</v>
       </c>
     </row>
     <row r="54">
@@ -58000,10 +58000,10 @@
         <v>185718</v>
       </c>
       <c r="N54" t="n">
-        <v>271</v>
+        <v>433</v>
       </c>
       <c r="O54" t="n">
-        <v>185989</v>
+        <v>186151</v>
       </c>
     </row>
     <row r="55">
@@ -58035,10 +58035,10 @@
         <v>137388</v>
       </c>
       <c r="N55" t="n">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="O55" t="n">
-        <v>137465</v>
+        <v>137518</v>
       </c>
     </row>
     <row r="56">
@@ -58066,10 +58066,10 @@
         <v>137812</v>
       </c>
       <c r="N56" t="n">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="O56" t="n">
-        <v>137915</v>
+        <v>137990</v>
       </c>
     </row>
     <row r="57">

</xml_diff>